<commit_message>
Adding stuff for lessons.
</commit_message>
<xml_diff>
--- a/Lesson 1 - Intro to Excel/First Notebook.xlsx
+++ b/Lesson 1 - Intro to Excel/First Notebook.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltwardos/git/data_analytics/Lesson 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltwardos/git/data_analytics/Lesson 1 - Intro to Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="460" windowWidth="27480" windowHeight="16820" tabRatio="500"/>
+    <workbookView xWindow="1320" yWindow="460" windowWidth="20440" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Item</t>
   </si>
@@ -43,15 +44,49 @@
   <si>
     <t>Random Weight</t>
   </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Volatility</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -74,13 +109,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -244,61 +283,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="1">
-                  <c:v>6.156025872935212</c:v>
+                  <c:v>11.29906097162509</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.94037129605395</c:v>
+                  <c:v>13.95394802309825</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.61326368841742</c:v>
+                  <c:v>11.90879994724413</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.21989561604911</c:v>
+                  <c:v>17.25567575749646</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.40436894786908</c:v>
+                  <c:v>27.21003437307444</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.1354424212922</c:v>
+                  <c:v>17.96793359195606</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>38.49067574140884</c:v>
+                  <c:v>36.84343205147962</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24.09164274295396</c:v>
+                  <c:v>21.71607223308823</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>39.407567642322</c:v>
+                  <c:v>41.30990441756731</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>37.76174230409827</c:v>
+                  <c:v>30.5064349516159</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>44.82292502246277</c:v>
+                  <c:v>45.38933556182593</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>35.76217460061271</c:v>
+                  <c:v>44.7825705807772</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42.86404315041392</c:v>
+                  <c:v>46.9180814800441</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>55.67600995264907</c:v>
+                  <c:v>57.70509949388177</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>56.75645540097473</c:v>
+                  <c:v>69.22403843993827</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>78.59492892754803</c:v>
+                  <c:v>56.24657454052322</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>83.51232306509623</c:v>
+                  <c:v>65.11650547909543</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>90.96036929738602</c:v>
+                  <c:v>94.46501801278922</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>87.3884664100604</c:v>
+                  <c:v>98.61712377561266</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -313,11 +352,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1825728720"/>
-        <c:axId val="1828364528"/>
+        <c:axId val="-2142875888"/>
+        <c:axId val="-2142869216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1825728720"/>
+        <c:axId val="-2142875888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -373,12 +412,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1828364528"/>
+        <c:crossAx val="-2142869216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1828364528"/>
+        <c:axId val="-2142869216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -435,7 +474,360 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1825728720"/>
+        <c:crossAx val="-2142875888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Value</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.702530731330446</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.397559412499124</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.491628451085938</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.20469905340467</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.90840221882599</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36.87243192470383</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>53.82543724595329</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>82.85322253424212</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>95.08249221735323</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>94.81648501026744</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95.99160667220475</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2105039232"/>
+        <c:axId val="-2007314096"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2105039232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2007314096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2007314096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2105039232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -524,7 +916,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1058,6 +2006,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1340,7 +2323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -1369,7 +2352,7 @@
       </c>
       <c r="B2">
         <f ca="1">RAND()</f>
-        <v>0.19853419576450704</v>
+        <v>0.36996869905416974</v>
       </c>
       <c r="C2">
         <f>A2^2</f>
@@ -1377,7 +2360,7 @@
       </c>
       <c r="D2">
         <f ca="1">($C2+$H$2*$B2)*$I$2</f>
-        <v>6.1560258729352118</v>
+        <v>11.299060971625092</v>
       </c>
       <c r="H2">
         <v>150</v>
@@ -1392,7 +2375,7 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B20" ca="1" si="0">RAND()</f>
-        <v>0.23801237653513163</v>
+        <v>0.43846493410327492</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C20" si="1">A3^2</f>
@@ -1400,7 +2383,7 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D20" ca="1" si="2">($C3+$H$2*$B3)*$I$2</f>
-        <v>7.9403712960539501</v>
+        <v>13.953948023098247</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1409,7 +2392,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5937754562805807</v>
+        <v>0.33695999824147083</v>
       </c>
       <c r="C4">
         <f t="shared" si="1"/>
@@ -1417,7 +2400,7 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="2"/>
-        <v>19.613263688417423</v>
+        <v>11.908799947244127</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1426,7 +2409,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33399652053497031</v>
+        <v>0.46852252524988214</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
@@ -1434,7 +2417,7 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="2"/>
-        <v>13.21989561604911</v>
+        <v>17.255675757496466</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1443,7 +2426,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48014563159563606</v>
+        <v>0.74033447910248118</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
@@ -1451,7 +2434,7 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="2"/>
-        <v>19.404368947869084</v>
+        <v>27.210034373074439</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1460,7 +2443,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.39784808070973987</v>
+        <v>0.35893111973186864</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
@@ -1468,7 +2451,7 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="2"/>
-        <v>19.135442421292197</v>
+        <v>17.967933591956058</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1477,7 +2460,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.95635585804696144</v>
+        <v>0.90144773504932074</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
@@ -1485,7 +2468,7 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="2"/>
-        <v>38.490675741408843</v>
+        <v>36.843432051479624</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1494,7 +2477,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37638809143179863</v>
+        <v>0.29720240776960749</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
@@ -1502,7 +2485,7 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="2"/>
-        <v>24.091642742953962</v>
+        <v>21.716072233088227</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1511,7 +2494,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.77358558807739985</v>
+        <v>0.83699681391891023</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
@@ -1519,7 +2502,7 @@
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="2"/>
-        <v>39.407567642322</v>
+        <v>41.30990441756731</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1528,7 +2511,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59205807680327549</v>
+        <v>0.35021449838719676</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
@@ -1536,7 +2519,7 @@
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="2"/>
-        <v>37.76174230409827</v>
+        <v>30.506434951615905</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1545,7 +2528,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.68743083408209216</v>
+        <v>0.70631118539419746</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
@@ -1553,7 +2536,7 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="2"/>
-        <v>44.822925022462769</v>
+        <v>45.389335561825931</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1562,7 +2545,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23207248668709024</v>
+        <v>0.53275235269257337</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
@@ -1570,7 +2553,7 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="2"/>
-        <v>35.76217460061271</v>
+        <v>44.782570580777204</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1579,7 +2562,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30213477168046388</v>
+        <v>0.43726938266813653</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
@@ -1587,7 +2570,7 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="2"/>
-        <v>42.86404315041392</v>
+        <v>46.918081480044101</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1596,7 +2579,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54920033175496896</v>
+        <v>0.61683664979605879</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
@@ -1604,7 +2587,7 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="2"/>
-        <v>55.676009952649068</v>
+        <v>57.705099493881768</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1613,7 +2596,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3918818466991576</v>
+        <v>0.80746794799794253</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
@@ -1621,7 +2604,7 @@
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="2"/>
-        <v>56.756455400974737</v>
+        <v>69.224038439938269</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1630,7 +2613,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91316429758493478</v>
+        <v>0.16821915135077414</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
@@ -1638,7 +2621,7 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="2"/>
-        <v>78.59492892754804</v>
+        <v>56.246574540523227</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1647,7 +2630,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85707743550320781</v>
+        <v>0.24388351596984781</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
@@ -1655,7 +2638,7 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="2"/>
-        <v>83.51232306509624</v>
+        <v>65.116505479095437</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1664,7 +2647,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87201230991286727</v>
+        <v>0.98883393375964024</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
@@ -1672,7 +2655,7 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="2"/>
-        <v>90.960369297386023</v>
+        <v>94.465018012789216</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1681,7 +2664,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.50628221366868009</v>
+        <v>0.88057079252042225</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
@@ -1689,7 +2672,286 @@
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="2"/>
-        <v>87.388466410060403</v>
+        <v>98.617123775612669</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>A2^2</f>
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4.2178855507426505E-3</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D12" si="0">B2*(2*(C2-0.5)*$F$2+1)</f>
+        <v>0.70253073133044563</v>
+      </c>
+      <c r="E2">
+        <f>ROUND(D2, 1)</f>
+        <v>0.7</v>
+      </c>
+      <c r="F2">
+        <v>0.3</v>
+      </c>
+      <c r="H2">
+        <f>COUNT(D2:D12)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B12" si="1">A3^2</f>
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>0.24898308854130158</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>3.397559412499124</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E4" si="2">ROUND(D3, 1)</f>
+        <v>3.4</v>
+      </c>
+      <c r="H3">
+        <f>MEDIAN(D2:D12)</f>
+        <v>36.872431924703832</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>3.5486750201099815E-2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>6.4916284510859388</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>6.5</v>
+      </c>
+      <c r="H4">
+        <f>AVERAGE(D2:D12)</f>
+        <v>45.740590497442803</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>0.31298948472965293</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>14.204699053404669</v>
+      </c>
+      <c r="E5">
+        <f>ROUND(D5, 1)</f>
+        <v>14.2</v>
+      </c>
+      <c r="H5">
+        <f>MAX(D2:D12)</f>
+        <v>95.991606672204753</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>9.3893481255066136E-2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>18.908402218825991</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E12" si="3">ROUND(D6, 1)</f>
+        <v>18.899999999999999</v>
+      </c>
+      <c r="H6">
+        <f>MIN(D2:D12)</f>
+        <v>0.70253073133044563</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="C7">
+        <v>0.54039036688443676</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>36.872431924703832</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>36.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="C8">
+        <v>0.66413051856983962</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>53.825437245953289</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>53.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="C9">
+        <v>0.99096933682922206</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>82.853222534242121</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>82.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+      <c r="C10">
+        <v>0.78976321434883201</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>95.082492217353234</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>95.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>0.41360808350445744</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>94.816485010267442</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>94.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="C12">
+        <v>0.15553177234441795</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>95.991606672204753</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>